<commit_message>
All file - slight stable version
Approved By sir, stable 19-09-2017
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -8,13 +8,15 @@
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="63">
   <si>
     <t>I131</t>
   </si>
@@ -98,6 +100,111 @@
   </si>
   <si>
     <t xml:space="preserve"> Total Number Density</t>
+  </si>
+  <si>
+    <t>I-131</t>
+  </si>
+  <si>
+    <t>I-132</t>
+  </si>
+  <si>
+    <t>I-133</t>
+  </si>
+  <si>
+    <t>I-134</t>
+  </si>
+  <si>
+    <t>I-135</t>
+  </si>
+  <si>
+    <t>Cs-134</t>
+  </si>
+  <si>
+    <t>Cs-137</t>
+  </si>
+  <si>
+    <t>Rb-88</t>
+  </si>
+  <si>
+    <t>Ru-103</t>
+  </si>
+  <si>
+    <t>Ru-106</t>
+  </si>
+  <si>
+    <t>Sr-89</t>
+  </si>
+  <si>
+    <t>Sr-90</t>
+  </si>
+  <si>
+    <t>Ce-141</t>
+  </si>
+  <si>
+    <t>Ce-144</t>
+  </si>
+  <si>
+    <t>Te-131m</t>
+  </si>
+  <si>
+    <t>Te-132</t>
+  </si>
+  <si>
+    <t>Ba-140</t>
+  </si>
+  <si>
+    <t>Zr-95</t>
+  </si>
+  <si>
+    <t>La-140</t>
+  </si>
+  <si>
+    <t>Kr-85</t>
+  </si>
+  <si>
+    <t>Kr-85m</t>
+  </si>
+  <si>
+    <t>Kr-87</t>
+  </si>
+  <si>
+    <t>Kr-88</t>
+  </si>
+  <si>
+    <t>Xe-133</t>
+  </si>
+  <si>
+    <t>Xe-135</t>
+  </si>
+  <si>
+    <t>Np238</t>
+  </si>
+  <si>
+    <t>Np239</t>
+  </si>
+  <si>
+    <t>Cm242</t>
+  </si>
+  <si>
+    <t>Cm244</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Lembda</t>
+  </si>
+  <si>
+    <t>Core InventoryS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Core inv </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Before cooling </t>
+  </si>
+  <si>
+    <t xml:space="preserve">After cooling </t>
   </si>
 </sst>
 </file>
@@ -406,7 +513,7 @@
   <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G21" sqref="G21"/>
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -462,7 +569,7 @@
         <v>1.96E+18</v>
       </c>
       <c r="F2">
-        <f t="shared" ref="F2:G22" si="1">E2/D2</f>
+        <f t="shared" ref="F2:F22" si="1">E2/D2</f>
         <v>2.3418181818181799E+22</v>
       </c>
     </row>
@@ -959,4 +1066,767 @@
   </sheetData>
   <pageMargins left="0.69930555555555596" right="0.69930555555555596" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:E34"/>
+  <sheetViews>
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="1">
+        <v>1.00010390689941E-6</v>
+      </c>
+      <c r="C1" s="1">
+        <v>1.48E+18</v>
+      </c>
+      <c r="D1">
+        <f>(C1/B1)</f>
+        <v>1.4798462337662457E+24</v>
+      </c>
+      <c r="E1">
+        <f>SUM(D1:D5)</f>
+        <v>1.8653259740259863E+24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>29</v>
+      </c>
+      <c r="B2" s="1">
+        <v>8.3695652173912995E-5</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1.96E+18</v>
+      </c>
+      <c r="D2">
+        <f t="shared" ref="D2:D33" si="0">(C2/B2)</f>
+        <v>2.3418181818181833E+22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B3" s="1">
+        <v>9.2548076923076892E-6</v>
+      </c>
+      <c r="C3" s="1">
+        <v>2.54E+18</v>
+      </c>
+      <c r="D3">
+        <f t="shared" si="0"/>
+        <v>2.7445194805194814E+23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4">
+        <v>2.19999999999999E-4</v>
+      </c>
+      <c r="C4" s="1">
+        <v>2.53E+18</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>1.1500000000000051E+22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5">
+      <c r="A5" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1">
+        <v>2.92998477929984E-5</v>
+      </c>
+      <c r="C5" s="1">
+        <v>2.23E+18</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>7.6109610389610592E+22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" s="1">
+        <v>1.06306604815551E-8</v>
+      </c>
+      <c r="C6" s="1">
+        <v>9.65E+16</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>9.0775168831168946E+24</v>
+      </c>
+      <c r="E6">
+        <f>SUM(D6:D7)</f>
+        <v>1.4591554285714288E+26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5">
+      <c r="A7" t="s">
+        <v>34</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7.3079101578812299E-10</v>
+      </c>
+      <c r="C7" s="1">
+        <v>1E+17</v>
+      </c>
+      <c r="D7">
+        <f t="shared" si="0"/>
+        <v>1.3683802597402598E+26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5">
+      <c r="A8" t="s">
+        <v>35</v>
+      </c>
+      <c r="B8">
+        <v>6.49606299212598E-4</v>
+      </c>
+      <c r="C8" s="1">
+        <v>5.22E+17</v>
+      </c>
+      <c r="D8">
+        <f t="shared" si="0"/>
+        <v>8.035636363636369E+20</v>
+      </c>
+      <c r="E8">
+        <v>8.035636363636369E+20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5">
+      <c r="A9" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="1">
+        <v>2.04300390558668E-7</v>
+      </c>
+      <c r="C9" s="1">
+        <v>2.41E+18</v>
+      </c>
+      <c r="D9">
+        <f t="shared" si="0"/>
+        <v>1.1796355324675365E+25</v>
+      </c>
+      <c r="E9">
+        <f>SUM(D9:D10)</f>
+        <v>6.116845714285729E+25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" t="s">
+        <v>37</v>
+      </c>
+      <c r="B10" s="1">
+        <v>2.1469614639934999E-8</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.06E+18</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="0"/>
+        <v>4.9372101818181922E+25</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5">
+      <c r="A11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B11" s="1">
+        <v>1.58734085361831E-7</v>
+      </c>
+      <c r="C11" s="1">
+        <v>7.12E+17</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="0"/>
+        <v>4.4854890389610462E+24</v>
+      </c>
+      <c r="E11">
+        <f>SUM(D11:D12)</f>
+        <v>4.2217289142857192E+25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5">
+      <c r="A12" t="s">
+        <v>39</v>
+      </c>
+      <c r="B12" s="1">
+        <v>7.6328189804615603E-10</v>
+      </c>
+      <c r="C12" s="1">
+        <v>2.88E+16</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="0"/>
+        <v>3.7731800103896148E+25</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" t="s">
+        <v>40</v>
+      </c>
+      <c r="B13" s="1">
+        <v>2.4679487179487101E-7</v>
+      </c>
+      <c r="C13" s="1">
+        <v>2.11E+18</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>8.5496103896104171E+24</v>
+      </c>
+      <c r="E13">
+        <f>SUM(D13:D14)</f>
+        <v>4.5844301298701407E+25</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5">
+      <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" s="1">
+        <v>2.8154141364503199E-8</v>
+      </c>
+      <c r="C14" s="1">
+        <v>1.05E+18</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="0"/>
+        <v>3.7294690909090988E+25</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5">
+      <c r="A15" t="s">
+        <v>42</v>
+      </c>
+      <c r="B15" s="1">
+        <v>6.4166666666666597E-6</v>
+      </c>
+      <c r="C15" s="1">
+        <v>1.63E+17</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="0"/>
+        <v>2.5402597402597428E+22</v>
+      </c>
+      <c r="E15">
+        <f>SUM(D15:D16)</f>
+        <v>7.7544935064935268E+23</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5">
+      <c r="A16" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="1">
+        <v>2.50651041666666E-6</v>
+      </c>
+      <c r="C16" s="1">
+        <v>1.88E+18</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="0"/>
+        <v>7.5004675324675526E+23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5">
+      <c r="A17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B17" s="1">
+        <v>6.2908496732026097E-7</v>
+      </c>
+      <c r="C17" s="1">
+        <v>1.93E+18</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="0"/>
+        <v>3.067948051948054E+24</v>
+      </c>
+      <c r="E17">
+        <v>3.067948051948054E+24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" s="1">
+        <v>1.25286368843069E-7</v>
+      </c>
+      <c r="C18" s="1">
+        <v>1.76E+18</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="0"/>
+        <v>1.404781714285724E+25</v>
+      </c>
+      <c r="E18">
+        <v>1.404781714285724E+25</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5">
+      <c r="A19" t="s">
+        <v>46</v>
+      </c>
+      <c r="B19" s="1">
+        <v>4.7743055555555504E-6</v>
+      </c>
+      <c r="C19" s="1">
+        <v>1.96E+18</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="0"/>
+        <v>4.1053090909090952E+23</v>
+      </c>
+      <c r="E19">
+        <v>4.1053090909090952E+23</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="1">
+        <v>2.0537276490419402E-9</v>
+      </c>
+      <c r="C20" s="1">
+        <v>4690000000000000</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="0"/>
+        <v>2.2836523636363739E+24</v>
+      </c>
+      <c r="E20">
+        <f>SUM(D20:D23)</f>
+        <v>2.2988953766233868E+24</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5">
+      <c r="A21" t="s">
+        <v>48</v>
+      </c>
+      <c r="B21" s="1">
+        <v>4.2968749999999998E-5</v>
+      </c>
+      <c r="C21" s="1">
+        <v>2.26E+17</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="0"/>
+        <v>5.259636363636364E+21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5">
+      <c r="A22" t="s">
+        <v>49</v>
+      </c>
+      <c r="B22">
+        <v>1.5137614678899E-4</v>
+      </c>
+      <c r="C22" s="1">
+        <v>4.08E+17</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="0"/>
+        <v>2.6952727272727422E+21</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5">
+      <c r="A23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B23" s="1">
+        <v>6.7781690140845006E-5</v>
+      </c>
+      <c r="C23" s="1">
+        <v>4.94E+17</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="0"/>
+        <v>7.288103896103903E+21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5">
+      <c r="A24" t="s">
+        <v>51</v>
+      </c>
+      <c r="B24" s="1">
+        <v>1.5306933842239099E-6</v>
+      </c>
+      <c r="C24" s="1">
+        <v>2.55E+18</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="0"/>
+        <v>1.6659116883116978E+24</v>
+      </c>
+      <c r="E24">
+        <f>SUM(D24:D25)</f>
+        <v>1.7922098701298798E+24</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5">
+      <c r="A25" t="s">
+        <v>52</v>
+      </c>
+      <c r="B25" s="1">
+        <v>2.1061269146608301E-5</v>
+      </c>
+      <c r="C25" s="1">
+        <v>2.66E+18</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="0"/>
+        <v>1.262981818181819E+23</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5">
+      <c r="A26" t="s">
+        <v>18</v>
+      </c>
+      <c r="B26" s="1">
+        <v>1.1882716049382701E-6</v>
+      </c>
+      <c r="C26" s="1">
+        <v>1.46E+17</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="0"/>
+        <v>1.2286753246753263E+23</v>
+      </c>
+      <c r="E26">
+        <v>1.2286753246753263E+23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5">
+      <c r="A27" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="1">
+        <v>3.7834119496855301E-6</v>
+      </c>
+      <c r="C27" s="1">
+        <v>5.39E+16</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="0"/>
+        <v>1.4246400000000017E+22</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5">
+      <c r="A28" t="s">
+        <v>54</v>
+      </c>
+      <c r="B28" s="1">
+        <v>3.4131205673758799E-6</v>
+      </c>
+      <c r="C28" s="1">
+        <v>2.59E+19</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="0"/>
+        <v>7.5883636363636507E+24</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5">
+      <c r="A29" t="s">
+        <v>19</v>
+      </c>
+      <c r="B29" s="1">
+        <v>9.00610075604461E-13</v>
+      </c>
+      <c r="C29" s="1">
+        <v>2170000000000000</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="0"/>
+        <v>2.4094778181818192E+27</v>
+      </c>
+      <c r="E29">
+        <f>SUM(D29:D31)</f>
+        <v>3.7571740114285741E+27</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5">
+      <c r="A30" t="s">
+        <v>20</v>
+      </c>
+      <c r="B30" s="1">
+        <v>3.3493195922494799E-12</v>
+      </c>
+      <c r="C30" s="1">
+        <v>3870000000000000</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="0"/>
+        <v>1.1554585620779232E+27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5">
+      <c r="A31" t="s">
+        <v>21</v>
+      </c>
+      <c r="B31" s="1">
+        <v>1.53455906737073E-9</v>
+      </c>
+      <c r="C31" s="1">
+        <v>2.95E+17</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="0"/>
+        <v>1.9223763116883121E+26</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5">
+      <c r="A32" t="s">
+        <v>55</v>
+      </c>
+      <c r="B32" s="1">
+        <v>4.9268018018017999E-8</v>
+      </c>
+      <c r="C32" s="1">
+        <v>8.16E+16</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="0"/>
+        <v>1.6562468571428578E+24</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>56</v>
+      </c>
+      <c r="B33" s="1">
+        <v>1.2140820908700999E-9</v>
+      </c>
+      <c r="C33" s="1">
+        <v>2700000000000000</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>2.2239023376623427E+24</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>57</v>
+      </c>
+      <c r="B34" t="s">
+        <v>58</v>
+      </c>
+      <c r="C34" t="s">
+        <v>59</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:C15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.85546875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C1" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1">
+        <v>2.2988999999999999E+24</v>
+      </c>
+      <c r="B2" s="1">
+        <v>2.299E+19</v>
+      </c>
+      <c r="C2" s="1">
+        <v>2.299E+19</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1">
+        <v>8.03564E+20</v>
+      </c>
+      <c r="B3" s="1">
+        <v>8036000000000000</v>
+      </c>
+      <c r="C3" s="1">
+        <v>8036000000000000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="1">
+        <v>4.2217299999999999E+25</v>
+      </c>
+      <c r="B4" s="1">
+        <v>4.222E+20</v>
+      </c>
+      <c r="C4" s="1">
+        <v>4.222E+20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1">
+        <v>1.4047800000000001E+25</v>
+      </c>
+      <c r="B5" s="1">
+        <v>8958</v>
+      </c>
+      <c r="C5" s="1">
+        <v>0.4365</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="1">
+        <v>6.1168499999999998E+25</v>
+      </c>
+      <c r="B6" s="1">
+        <v>166.4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1.5839999999999999E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1">
+        <v>7.7544900000000005E+23</v>
+      </c>
+      <c r="B7" s="1">
+        <v>7.754E+18</v>
+      </c>
+      <c r="C7" s="1">
+        <v>7.754E+18</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" s="1">
+        <v>1.86533E+24</v>
+      </c>
+      <c r="B8" s="1">
+        <v>1.865E+19</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1.865E+19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="1">
+        <v>1.79221E+24</v>
+      </c>
+      <c r="B9" s="1">
+        <v>1.792E+19</v>
+      </c>
+      <c r="C9" s="1">
+        <v>1.792E+19</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" s="1">
+        <v>1.45916E+21</v>
+      </c>
+      <c r="B10" s="1">
+        <v>1.459E+16</v>
+      </c>
+      <c r="C10" s="1">
+        <v>1.459E+16</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" s="1">
+        <v>3.0679500000000002E+24</v>
+      </c>
+      <c r="B11" s="1">
+        <v>3.068E+19</v>
+      </c>
+      <c r="C11" s="1">
+        <v>3.068E+19</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" s="1">
+        <v>4.1053099999999999E+23</v>
+      </c>
+      <c r="B12" s="1">
+        <v>3145000000</v>
+      </c>
+      <c r="C12" s="1">
+        <v>1959000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13" s="1">
+        <v>4.5844300000000002E+25</v>
+      </c>
+      <c r="B13" s="1">
+        <v>5168000000</v>
+      </c>
+      <c r="C13" s="1">
+        <v>4038000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14" s="1">
+        <v>1.2286799999999999E+23</v>
+      </c>
+      <c r="B14" s="1">
+        <v>1470000</v>
+      </c>
+      <c r="C14" s="1">
+        <v>181.1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15" s="1">
+        <v>3.7571700000000002E+27</v>
+      </c>
+      <c r="B15" s="1">
+        <v>216500000000</v>
+      </c>
+      <c r="C15" s="1">
+        <v>787700000</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>